<commit_message>
Se agrego grafico para estudiar la relacion entre densidad problacional y superficie afectada
</commit_message>
<xml_diff>
--- a/datasets/Superficie afectada por incendios reportados, por jurisdicción.xlsx
+++ b/datasets/Superficie afectada por incendios reportados, por jurisdicción.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fede4\OneDrive\Documents\UNRN\Ciencia de Datos - 25.1\Proyecto Final\Analisis_PrediccionIncendiosForestales\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0CF2AD4-B11F-46A4-8748-1A3F1BC26D4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AA277ED-6117-473C-8E2A-CDA52A33BF18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -460,7 +460,7 @@
   <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -956,7 +956,7 @@
       <c r="D14" s="1">
         <v>65022</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E14" s="9">
         <v>33345</v>
       </c>
       <c r="F14" s="1">

</xml_diff>

<commit_message>
Analisis de correlaciones profundas
</commit_message>
<xml_diff>
--- a/datasets/Superficie afectada por incendios reportados, por jurisdicción.xlsx
+++ b/datasets/Superficie afectada por incendios reportados, por jurisdicción.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fede4\OneDrive\Documents\UNRN\Ciencia de Datos - 25.1\Proyecto Final\Analisis_PrediccionIncendiosForestales\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AA277ED-6117-473C-8E2A-CDA52A33BF18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4D66FDC-E9B4-4F21-AA55-B4FE06EDAB49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -460,7 +460,7 @@
   <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>